<commit_message>
excel work study chairs
</commit_message>
<xml_diff>
--- a/src/test/resources/bookShelvesData.xlsx
+++ b/src/test/resources/bookShelvesData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cognizantonline-my.sharepoint.com/personal/2304139_cognizant_com/Documents/Documents/hackpro/hackpro/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{87A132FA-5C63-4F8A-A96B-F5E016F0D6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B4043F0-5E2A-4D11-B95B-B04099073B08}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{87A132FA-5C63-4F8A-A96B-F5E016F0D6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27A98444-E41E-488A-BA01-1349874AA4EE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{1EE71F21-BE0C-45B8-8C54-6BF7520E329B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{1EE71F21-BE0C-45B8-8C54-6BF7520E329B}"/>
   </bookViews>
   <sheets>
     <sheet name="BookShelves" sheetId="1" r:id="rId1"/>
     <sheet name="submenuItems" sheetId="2" r:id="rId2"/>
+    <sheet name="StudyChairs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>Model Name</t>
   </si>
@@ -100,12 +101,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -122,6 +125,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -430,18 +437,18 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="43.36328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.36328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="35.36328125" customWidth="1"/>
     <col min="3" max="3" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -455,7 +462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8CBD9F2-1631-40D5-A9A0-D30190E163F5}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -465,12 +472,43 @@
     <col min="2" max="2" width="31.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8643A83F-BA78-4CBB-91EF-DFA5D413D930}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.26953125" customWidth="1"/>
+    <col min="2" max="2" width="35" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all excel updates completed
</commit_message>
<xml_diff>
--- a/src/test/resources/bookShelvesData.xlsx
+++ b/src/test/resources/bookShelvesData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cognizantonline-my.sharepoint.com/personal/2304139_cognizant_com/Documents/Documents/hackpro/hackpro/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{87A132FA-5C63-4F8A-A96B-F5E016F0D6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27A98444-E41E-488A-BA01-1349874AA4EE}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{87A132FA-5C63-4F8A-A96B-F5E016F0D6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8A1AC4C-7448-42CF-BC98-17F86D90BEFB}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{1EE71F21-BE0C-45B8-8C54-6BF7520E329B}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
   <si>
     <t>Model Name</t>
   </si>
@@ -53,12 +53,37 @@
   </si>
   <si>
     <t>Living Storage Menu</t>
+  </si>
+  <si>
+    <t>By Urban Ladder</t>
+  </si>
+  <si>
+    <t>₹12,287</t>
+  </si>
+  <si>
+    <t>Galen Study Chair In Black Colour</t>
+  </si>
+  <si>
+    <t>₹7,505</t>
+  </si>
+  <si>
+    <t>Hawley Study Chair</t>
+  </si>
+  <si>
+    <t>₹6,440</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Mika Leatherette Study Chair In Scarlet Red Colour</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -125,10 +150,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -436,9 +457,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="43.36328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.36328125" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="43.36328125"/>
+    <col min="2" max="2" customWidth="true" width="35.36328125"/>
+    <col min="3" max="3" customWidth="true" width="17.453125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -468,8 +489,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.26953125" customWidth="1"/>
-    <col min="2" max="2" width="31.26953125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="35.26953125"/>
+    <col min="2" max="2" customWidth="true" width="31.26953125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -487,17 +508,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8643A83F-BA78-4CBB-91EF-DFA5D413D930}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.26953125" customWidth="1"/>
-    <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="26.1796875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="26.26953125"/>
+    <col min="2" max="2" customWidth="true" width="35.0"/>
+    <col min="3" max="3" customWidth="true" width="26.1796875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -511,6 +532,39 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ready to execute 4
</commit_message>
<xml_diff>
--- a/src/test/resources/bookShelvesData.xlsx
+++ b/src/test/resources/bookShelvesData.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="38">
   <si>
     <t>Model Name</t>
   </si>
@@ -77,6 +77,81 @@
   </si>
   <si>
     <t>Mika Leatherette Study Chair In Scarlet Red Colour</t>
+  </si>
+  <si>
+    <t>Rhodes Solid Wood Bookshelf In Mahogany Finish</t>
+  </si>
+  <si>
+    <t>₹14,755</t>
+  </si>
+  <si>
+    <t>Rhodes Solid Wood Bookshelf In Teak Finish</t>
+  </si>
+  <si>
+    <t>Theodore Engineered Wood Bookshelf In Rustic Walnut Finish</t>
+  </si>
+  <si>
+    <t>₹12,814</t>
+  </si>
+  <si>
+    <t>Lounge Chairs</t>
+  </si>
+  <si>
+    <t>Accent Chairs</t>
+  </si>
+  <si>
+    <t>Recliners</t>
+  </si>
+  <si>
+    <t>Sofa Cum Bed</t>
+  </si>
+  <si>
+    <t>UL Assured Picks</t>
+  </si>
+  <si>
+    <t>Ottomans &amp; Stools</t>
+  </si>
+  <si>
+    <t>Bean Bags</t>
+  </si>
+  <si>
+    <t>Benches</t>
+  </si>
+  <si>
+    <t>Bar Stools</t>
+  </si>
+  <si>
+    <t>Rocking Chairs</t>
+  </si>
+  <si>
+    <t>Gaming Chairs</t>
+  </si>
+  <si>
+    <t>TV Units</t>
+  </si>
+  <si>
+    <t>Bookshelves</t>
+  </si>
+  <si>
+    <t>Shoe Racks</t>
+  </si>
+  <si>
+    <t>Prayer Units</t>
+  </si>
+  <si>
+    <t>Showcases</t>
+  </si>
+  <si>
+    <t>Wall Shelves</t>
+  </si>
+  <si>
+    <t>Entryway &amp; Foyer</t>
+  </si>
+  <si>
+    <t>Room Divider</t>
+  </si>
+  <si>
+    <t>Living Room Sets</t>
   </si>
 </sst>
 </file>
@@ -449,7 +524,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{740B5915-A26E-4703-9C3E-E46B2E50FCAB}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
@@ -473,6 +548,39 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s" s="1">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="1">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="1">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -481,7 +589,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8CBD9F2-1631-40D5-A9A0-D30190E163F5}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -499,6 +607,88 @@
       </c>
       <c r="B1" s="3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -537,10 +727,10 @@
         <v>12</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>